<commit_message>
Project expenses: add note about jumper wires
</commit_message>
<xml_diff>
--- a/Dokumentit/projektikustannukset.xlsx
+++ b/Dokumentit/projektikustannukset.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>Ostaja</t>
   </si>
@@ -139,13 +139,31 @@
   </si>
   <si>
     <t>Kulu per ryhmäläinen</t>
+  </si>
+  <si>
+    <t>GPIO-johdot</t>
+  </si>
+  <si>
+    <t>Taustaa:</t>
+  </si>
+  <si>
+    <t>R2,54/2,0 HYPPYJOHTO N/N MONIVÄRILATTA 20cm 40pin</t>
+  </si>
+  <si>
+    <t>Partcon johtosetin mukana tulee 40 johtoa, joista projektissa käytössä on 34 johtoa (joko irtonaisina tai kytkettyinä)</t>
+  </si>
+  <si>
+    <t>Useiden antureiden mukana tuli omat johtonsa, kuinka paljon? Projektissa käytettiin myös Pekan aiemmin hommaamia johtoja (Partco)</t>
+  </si>
+  <si>
+    <t>Johdot ovat "sekaisin" projektin jäljiltä</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +193,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -199,10 +233,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -213,25 +248,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -531,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +582,7 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="44.875" customWidth="1"/>
     <col min="7" max="7" width="17.125" customWidth="1"/>
-    <col min="8" max="8" width="4.875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="4.875" style="8" customWidth="1"/>
     <col min="9" max="9" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -930,54 +969,54 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="10">
         <f>((2*14)/100 * 8 * 1.58)</f>
         <v>3.5392000000000006</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="6"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="9"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="10">
         <f>((2*15)/100 * 8 * 1.58)</f>
         <v>3.7919999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="6"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="9"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F21" s="4">
@@ -989,7 +1028,7 @@
       <c r="D23" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <f>SUM(F8,F21)</f>
         <v>76.051199999999994</v>
       </c>
@@ -1008,12 +1047,67 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="7" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="D19:D20"/>
@@ -1022,11 +1116,12 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A32" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>